<commit_message>
100cut FDR + wholegenome Bonferroni => done
</commit_message>
<xml_diff>
--- a/HNSCC_OS_marginS_candidates_Bonferroni.xlsx
+++ b/HNSCC_OS_marginS_candidates_Bonferroni.xlsx
@@ -12,18 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="88">
   <si>
     <t>Reported by Tex Li-Hsing Chi. 
 tex@gate.sinica.edu.tw 
 Cohort with surgical margins status (0 or 1)
-2020-03-08</t>
+2020-03-12</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve">Table 1. The 10 candiate genes overexpressed and worsed prognosis in HNSCC (ranked by Bonferroni corrected Kaplan Meier P-value) 
+    <t xml:space="preserve">Table 1. The 10 candiate genes overexpressed with poor prognosis in HNSCC (ranked by Bonferroni corrected Kaplan Meier P-value) 
 </t>
   </si>
   <si>
@@ -168,10 +168,6 @@
     <t>Selection criteria: 
  Bonferroni KM P-value &lt; 0.05 
  Cox's univariate &amp; multivariate HR &gt;= 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table 2. The 10 candiate genes overexpressed and better prognosis in HNSCC (ranked by Bonferroni corrected Kaplan Meier P-value) 
-</t>
   </si>
   <si>
     <t xml:space="preserve">Table 2. The 10 candiate genes overexpressed with better prognosis in HNSCC (ranked by Bonferroni corrected Kaplan Meier P-value) 
@@ -296,7 +292,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="40">
+  <fonts count="34">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -404,49 +400,6 @@
       <name val="Calibri"/>
       <sz val="14.0"/>
       <color rgb="00008B"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="22.0"/>
-      <color rgb="000000"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="18.0"/>
-      <color rgb="000000"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="16.0"/>
-      <color rgb="000000"/>
-      <i val="true"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="16.0"/>
-      <color rgb="000000"/>
-      <i val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="14.0"/>
-      <color rgb="000000"/>
-      <i val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color rgb="000000"/>
-      <i val="true"/>
-      <u val="none"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -586,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -643,34 +596,22 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
       <alignment horizontal="center" wrapText="true"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="justify" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -721,14 +662,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>388938</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>875166</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -746,7 +687,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6924675" cy="5857875"/>
+          <a:ext cx="5543550" cy="4648200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1292,302 +1233,302 @@
       </c>
     </row>
     <row r="58">
-      <c r="B58" t="s" s="53">
+      <c r="B58"/>
+      <c r="C58" t="s" s="49">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s" s="49">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s" s="49">
+        <v>5</v>
+      </c>
+      <c r="F58" t="s" s="49">
+        <v>6</v>
+      </c>
+      <c r="G58" t="s" s="49">
+        <v>7</v>
+      </c>
+      <c r="H58" t="s" s="49">
+        <v>8</v>
+      </c>
+      <c r="I58" t="s" s="49">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s" s="45">
         <v>51</v>
       </c>
-    </row>
-    <row r="59">
-      <c r="B59"/>
-      <c r="C59" t="s" s="61">
-        <v>3</v>
-      </c>
-      <c r="D59" t="s" s="61">
-        <v>4</v>
-      </c>
-      <c r="E59" t="s" s="61">
-        <v>5</v>
-      </c>
-      <c r="F59" t="s" s="61">
-        <v>6</v>
-      </c>
-      <c r="G59" t="s" s="61">
-        <v>7</v>
-      </c>
-      <c r="H59" t="s" s="61">
-        <v>8</v>
-      </c>
-      <c r="I59" t="s" s="61">
-        <v>9</v>
+      <c r="C59" t="s" s="50">
+        <v>61</v>
+      </c>
+      <c r="D59" t="s" s="51">
+        <v>71</v>
+      </c>
+      <c r="E59" t="s" s="52">
+        <v>40</v>
+      </c>
+      <c r="F59" t="n" s="53">
+        <v>0.465</v>
+      </c>
+      <c r="G59" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H59" t="n" s="55">
+        <v>0.499</v>
+      </c>
+      <c r="I59" t="n" s="56">
+        <v>0.0</v>
       </c>
     </row>
     <row r="60">
-      <c r="B60" t="s" s="57">
+      <c r="B60" t="s" s="45">
         <v>52</v>
       </c>
-      <c r="C60" t="s" s="62">
+      <c r="C60" t="s" s="50">
         <v>62</v>
       </c>
-      <c r="D60" t="s" s="63">
+      <c r="D60" t="s" s="51">
         <v>72</v>
       </c>
-      <c r="E60" t="s" s="64">
+      <c r="E60" t="s" s="52">
         <v>40</v>
       </c>
-      <c r="F60" t="n" s="65">
-        <v>0.465</v>
-      </c>
-      <c r="G60" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H60" t="n" s="67">
+      <c r="F60" t="n" s="53">
+        <v>0.474</v>
+      </c>
+      <c r="G60" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H60" t="n" s="55">
+        <v>0.453</v>
+      </c>
+      <c r="I60" t="n" s="56">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s" s="45">
+        <v>53</v>
+      </c>
+      <c r="C61" t="s" s="50">
+        <v>63</v>
+      </c>
+      <c r="D61" t="s" s="51">
+        <v>73</v>
+      </c>
+      <c r="E61" t="s" s="52">
+        <v>41</v>
+      </c>
+      <c r="F61" t="n" s="53">
+        <v>0.472</v>
+      </c>
+      <c r="G61" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H61" t="n" s="55">
+        <v>0.459</v>
+      </c>
+      <c r="I61" t="n" s="56">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s" s="45">
+        <v>54</v>
+      </c>
+      <c r="C62" t="s" s="50">
+        <v>64</v>
+      </c>
+      <c r="D62" t="s" s="51">
+        <v>74</v>
+      </c>
+      <c r="E62" t="s" s="52">
+        <v>81</v>
+      </c>
+      <c r="F62" t="n" s="53">
+        <v>0.468</v>
+      </c>
+      <c r="G62" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H62" t="n" s="55">
+        <v>0.467</v>
+      </c>
+      <c r="I62" t="n" s="56">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s" s="45">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s" s="50">
+        <v>65</v>
+      </c>
+      <c r="D63" t="s" s="51">
+        <v>75</v>
+      </c>
+      <c r="E63" t="s" s="52">
+        <v>82</v>
+      </c>
+      <c r="F63" t="n" s="53">
+        <v>0.484</v>
+      </c>
+      <c r="G63" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H63" t="n" s="55">
+        <v>0.496</v>
+      </c>
+      <c r="I63" t="n" s="56">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s" s="45">
+        <v>56</v>
+      </c>
+      <c r="C64" t="s" s="50">
+        <v>66</v>
+      </c>
+      <c r="D64" t="s" s="51">
+        <v>76</v>
+      </c>
+      <c r="E64" t="s" s="52">
+        <v>83</v>
+      </c>
+      <c r="F64" t="n" s="53">
         <v>0.499</v>
       </c>
-      <c r="I60" t="n" s="68">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="B61" t="s" s="57">
-        <v>53</v>
-      </c>
-      <c r="C61" t="s" s="62">
-        <v>63</v>
-      </c>
-      <c r="D61" t="s" s="63">
-        <v>73</v>
-      </c>
-      <c r="E61" t="s" s="64">
-        <v>40</v>
-      </c>
-      <c r="F61" t="n" s="65">
-        <v>0.474</v>
-      </c>
-      <c r="G61" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H61" t="n" s="67">
-        <v>0.453</v>
-      </c>
-      <c r="I61" t="n" s="68">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="B62" t="s" s="57">
-        <v>54</v>
-      </c>
-      <c r="C62" t="s" s="62">
-        <v>64</v>
-      </c>
-      <c r="D62" t="s" s="63">
-        <v>74</v>
-      </c>
-      <c r="E62" t="s" s="64">
-        <v>41</v>
-      </c>
-      <c r="F62" t="n" s="65">
-        <v>0.472</v>
-      </c>
-      <c r="G62" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H62" t="n" s="67">
-        <v>0.459</v>
-      </c>
-      <c r="I62" t="n" s="68">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="B63" t="s" s="57">
-        <v>55</v>
-      </c>
-      <c r="C63" t="s" s="62">
-        <v>65</v>
-      </c>
-      <c r="D63" t="s" s="63">
-        <v>75</v>
-      </c>
-      <c r="E63" t="s" s="64">
-        <v>82</v>
-      </c>
-      <c r="F63" t="n" s="65">
-        <v>0.468</v>
-      </c>
-      <c r="G63" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H63" t="n" s="67">
-        <v>0.467</v>
-      </c>
-      <c r="I63" t="n" s="68">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="B64" t="s" s="57">
-        <v>56</v>
-      </c>
-      <c r="C64" t="s" s="62">
-        <v>66</v>
-      </c>
-      <c r="D64" t="s" s="63">
-        <v>76</v>
-      </c>
-      <c r="E64" t="s" s="64">
-        <v>83</v>
-      </c>
-      <c r="F64" t="n" s="65">
-        <v>0.484</v>
-      </c>
-      <c r="G64" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H64" t="n" s="67">
-        <v>0.496</v>
-      </c>
-      <c r="I64" t="n" s="68">
+      <c r="G64" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H64" t="n" s="55">
+        <v>0.485</v>
+      </c>
+      <c r="I64" t="n" s="56">
         <v>0.0</v>
       </c>
     </row>
     <row r="65">
-      <c r="B65" t="s" s="57">
+      <c r="B65" t="s" s="45">
         <v>57</v>
       </c>
-      <c r="C65" t="s" s="62">
+      <c r="C65" t="s" s="50">
         <v>67</v>
       </c>
-      <c r="D65" t="s" s="63">
+      <c r="D65" t="s" s="51">
         <v>77</v>
       </c>
-      <c r="E65" t="s" s="64">
+      <c r="E65" t="s" s="52">
         <v>84</v>
       </c>
-      <c r="F65" t="n" s="65">
+      <c r="F65" t="n" s="53">
+        <v>0.49</v>
+      </c>
+      <c r="G65" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H65" t="n" s="55">
+        <v>0.494</v>
+      </c>
+      <c r="I65" t="n" s="56">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s" s="45">
+        <v>58</v>
+      </c>
+      <c r="C66" t="s" s="50">
+        <v>68</v>
+      </c>
+      <c r="D66" t="s" s="51">
+        <v>78</v>
+      </c>
+      <c r="E66" t="s" s="52">
+        <v>45</v>
+      </c>
+      <c r="F66" t="n" s="53">
         <v>0.499</v>
       </c>
-      <c r="G65" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H65" t="n" s="67">
-        <v>0.485</v>
-      </c>
-      <c r="I65" t="n" s="68">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="B66" t="s" s="57">
-        <v>58</v>
-      </c>
-      <c r="C66" t="s" s="62">
-        <v>68</v>
-      </c>
-      <c r="D66" t="s" s="63">
-        <v>78</v>
-      </c>
-      <c r="E66" t="s" s="64">
+      <c r="G66" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H66" t="n" s="55">
+        <v>0.481</v>
+      </c>
+      <c r="I66" t="n" s="56">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s" s="45">
+        <v>59</v>
+      </c>
+      <c r="C67" t="s" s="50">
+        <v>69</v>
+      </c>
+      <c r="D67" t="s" s="51">
+        <v>79</v>
+      </c>
+      <c r="E67" t="s" s="52">
         <v>85</v>
       </c>
-      <c r="F66" t="n" s="65">
-        <v>0.49</v>
-      </c>
-      <c r="G66" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H66" t="n" s="67">
-        <v>0.494</v>
-      </c>
-      <c r="I66" t="n" s="68">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="B67" t="s" s="57">
-        <v>59</v>
-      </c>
-      <c r="C67" t="s" s="62">
-        <v>69</v>
-      </c>
-      <c r="D67" t="s" s="63">
-        <v>79</v>
-      </c>
-      <c r="E67" t="s" s="64">
-        <v>45</v>
-      </c>
-      <c r="F67" t="n" s="65">
-        <v>0.499</v>
-      </c>
-      <c r="G67" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H67" t="n" s="67">
-        <v>0.481</v>
-      </c>
-      <c r="I67" t="n" s="68">
+      <c r="F67" t="n" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="G67" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H67" t="n" s="55">
+        <v>0.483</v>
+      </c>
+      <c r="I67" t="n" s="56">
         <v>0.0</v>
       </c>
     </row>
     <row r="68">
-      <c r="B68" t="s" s="57">
+      <c r="B68" t="s" s="45">
         <v>60</v>
       </c>
-      <c r="C68" t="s" s="62">
+      <c r="C68" t="s" s="50">
         <v>70</v>
       </c>
-      <c r="D68" t="s" s="63">
+      <c r="D68" t="s" s="51">
         <v>80</v>
       </c>
-      <c r="E68" t="s" s="64">
+      <c r="E68" t="s" s="52">
         <v>86</v>
       </c>
-      <c r="F68" t="n" s="65">
-        <v>0.5</v>
-      </c>
-      <c r="G68" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H68" t="n" s="67">
-        <v>0.483</v>
-      </c>
-      <c r="I68" t="n" s="68">
+      <c r="F68" t="n" s="53">
+        <v>0.46</v>
+      </c>
+      <c r="G68" t="n" s="54">
+        <v>0.001</v>
+      </c>
+      <c r="H68" t="n" s="55">
+        <v>0.457</v>
+      </c>
+      <c r="I68" t="n" s="56">
         <v>0.0</v>
       </c>
     </row>
     <row r="69">
-      <c r="B69" t="s" s="57">
-        <v>61</v>
-      </c>
-      <c r="C69" t="s" s="62">
-        <v>71</v>
-      </c>
-      <c r="D69" t="s" s="63">
-        <v>81</v>
-      </c>
-      <c r="E69" t="s" s="64">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s" s="59">
         <v>87</v>
       </c>
-      <c r="F69" t="n" s="65">
-        <v>0.46</v>
-      </c>
-      <c r="G69" t="n" s="66">
-        <v>0.001</v>
-      </c>
-      <c r="H69" t="n" s="67">
-        <v>0.457</v>
-      </c>
-      <c r="I69" t="n" s="68">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="71">
-      <c r="B71" t="s" s="71">
-        <v>88</v>
+      <c r="A71" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -1752,11 +1693,6 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1764,7 +1700,7 @@
   <mergeCells>
     <mergeCell ref="B1:F4"/>
     <mergeCell ref="B47:E50"/>
-    <mergeCell ref="B71:E74"/>
+    <mergeCell ref="B70:E73"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>

</xml_diff>